<commit_message>
Fix csv/xls unicode support
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="220" yWindow="220" windowWidth="21360" windowHeight="14360" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test.csv" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Some Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,6 +34,20 @@
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Sparse Data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unicode Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iñtërnâtiônàližætiøn</t>
+  </si>
+  <si>
+    <t>Ādam</t>
+  </si>
 </sst>
 </file>
 
@@ -45,8 +59,8 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="166" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="167" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="168" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -81,8 +95,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,84 +494,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>30075</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
         <v>234</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>42005</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2"/>
+      <c r="C3">
         <v>100</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>35064</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3"/>
+      <c r="C4">
         <v>0.44</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
       <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -577,6 +610,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -594,6 +628,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <sheetData/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>